<commit_message>
rename output files for clarity
</commit_message>
<xml_diff>
--- a/output/biden_shared_donors.xlsx
+++ b/output/biden_shared_donors.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B184"/>
+  <dimension ref="A1:B194"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -372,19 +372,19 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BENNET, MICHAEL F.</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ANDY SPAHN</t>
+          <t>ANDREW WEINSTEIN</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>BENNET, MICHAEL F.</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -396,7 +396,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>BOOKER, CORY A.</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -408,7 +408,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>BUTTIGIEG, PETE</t>
+          <t>BOOKER, CORY A.</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -420,7 +420,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>KLOBUCHAR, AMY J.</t>
+          <t>BUTTIGIEG, PETE</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -432,12 +432,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>KLOBUCHAR, AMY J.</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>AZITA RAJI</t>
+          <t>ANDY SPAHN</t>
         </is>
       </c>
     </row>
@@ -449,7 +449,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>BARRY GOODMAN</t>
+          <t>AZITA RAJI</t>
         </is>
       </c>
     </row>
@@ -461,14 +461,14 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>BILL STETSON</t>
+          <t>BARRY GOODMAN</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>BUTTIGIEG, PETE</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -480,7 +480,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>KLOBUCHAR, AMY J.</t>
+          <t>BUTTIGIEG, PETE</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -492,19 +492,19 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>BENNET, MICHAEL F.</t>
+          <t>KLOBUCHAR, AMY J.</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>BLAIR EFFRON</t>
+          <t>BILL STETSON</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>BENNET, MICHAEL F.</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -516,7 +516,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>BOOKER, CORY A.</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -528,7 +528,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>GILLIBRAND, KIRSTEN</t>
+          <t>BOOKER, CORY A.</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -540,7 +540,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>HARRIS, KAMALA D.</t>
+          <t>GILLIBRAND, KIRSTEN</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -552,7 +552,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>O'ROURKE, BETO</t>
+          <t>HARRIS, KAMALA D.</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -564,12 +564,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>O'ROURKE, BETO</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>BOB CLARK</t>
+          <t>BLAIR EFFRON</t>
         </is>
       </c>
     </row>
@@ -581,7 +581,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>BOB SHERMAN</t>
+          <t>BOB CLARK</t>
         </is>
       </c>
     </row>
@@ -593,19 +593,19 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>BOBBY STEIN</t>
+          <t>BOB SATAWAKE</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>BUTTIGIEG, PETE</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>CAROL FRILLMAN</t>
+          <t>BOB SATAWAKE</t>
         </is>
       </c>
     </row>
@@ -617,7 +617,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>CAROL HAMILTON</t>
+          <t>BOB SHERMAN</t>
         </is>
       </c>
     </row>
@@ -629,38 +629,38 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>CAROL PENSKY</t>
+          <t>BOBBY STEIN</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>BUTTIGIEG, PETE</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>CAROL PENSKY</t>
+          <t>CAROL FRILLMAN</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>GILLIBRAND, KIRSTEN</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>CAROL PENSKY</t>
+          <t>CAROL HAMILTON</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>HARRIS, KAMALA D.</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -672,60 +672,60 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>BUTTIGIEG, PETE</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>CARY PATTERSON</t>
+          <t>CAROL PENSKY</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>GILLIBRAND, KIRSTEN</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>CHARLES BONE</t>
+          <t>CAROL PENSKY</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>HARRIS, KAMALA D.</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>CHARLES MYERS</t>
+          <t>CAROL PENSKY</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>BULLOCK, STEVE</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>CHARLES MYERS</t>
+          <t>CARY PATTERSON</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>HARRIS, KAMALA D.</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>CHARLES MYERS</t>
+          <t>CHARLES BONE</t>
         </is>
       </c>
     </row>
@@ -737,50 +737,50 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>CHIP FORRESTER</t>
+          <t>CHARLES MYERS</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>BULLOCK, STEVE</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>CHRIS SACCA</t>
+          <t>CHARLES MYERS</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>BOOKER, CORY A.</t>
+          <t>HARRIS, KAMALA D.</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>CHRIS SACCA</t>
+          <t>CHARLES MYERS</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>BUTTIGIEG, PETE</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>CHRIS SACCA</t>
+          <t>CHIP FORRESTER</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>INSLEE, JAY R.</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -792,7 +792,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>WARREN, ELIZABETH</t>
+          <t>BOOKER, CORY A.</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -804,36 +804,36 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>BUTTIGIEG, PETE</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>CLIFF LEVINE</t>
+          <t>CHRIS SACCA</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>BULLOCK, STEVE</t>
+          <t>INSLEE, JAY R.</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>CLIFF LEVINE</t>
+          <t>CHRIS SACCA</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>WARREN, ELIZABETH</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>COLLEEN BELL</t>
+          <t>CHRIS SACCA</t>
         </is>
       </c>
     </row>
@@ -845,19 +845,19 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>COOKIE PARKER</t>
+          <t>CLIFF LEVINE</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>BULLOCK, STEVE</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>DAVID COHEN</t>
+          <t>CLIFF LEVINE</t>
         </is>
       </c>
     </row>
@@ -869,7 +869,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>DAVID GARRISON</t>
+          <t>COLLEEN BELL</t>
         </is>
       </c>
     </row>
@@ -881,19 +881,19 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>DENISE BAUER</t>
+          <t>COOKIE PARKER</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>BENNET, MICHAEL F.</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>DEVEN PAREKH</t>
+          <t>DAVID COHEN</t>
         </is>
       </c>
     </row>
@@ -905,26 +905,26 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>DEVEN PAREKH</t>
+          <t>DAVID GARRISON</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>BUTTIGIEG, PETE</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>DEVEN PAREKH</t>
+          <t>DENISE BAUER</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>GILLIBRAND, KIRSTEN</t>
+          <t>BENNET, MICHAEL F.</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -936,7 +936,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>HARRIS, KAMALA D.</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -948,60 +948,60 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>BUTTIGIEG, PETE</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>DOUG DUNHAM</t>
+          <t>DEVEN PAREKH</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>GILLIBRAND, KIRSTEN</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>DOUG HICKEY</t>
+          <t>DEVEN PAREKH</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>HARRIS, KAMALA D.</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>ELIZABETH BAGLEY</t>
+          <t>DEVEN PAREKH</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>HARRIS, KAMALA D.</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>ELIZABETH BAGLEY</t>
+          <t>DOUG DUNHAM</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>KLOBUCHAR, AMY J.</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>ELIZABETH BAGLEY</t>
+          <t>DOUG HICKEY</t>
         </is>
       </c>
     </row>
@@ -1013,50 +1013,50 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>ELLEN CHESLER</t>
+          <t>ELIZABETH BAGLEY</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>BENNET, MICHAEL F.</t>
+          <t>HARRIS, KAMALA D.</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>FRED EYCHANER</t>
+          <t>ELIZABETH BAGLEY</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>KLOBUCHAR, AMY J.</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>FRED EYCHANER</t>
+          <t>ELIZABETH BAGLEY</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>BUTTIGIEG, PETE</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>FRED EYCHANER</t>
+          <t>ELLEN CHESLER</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>KLOBUCHAR, AMY J.</t>
+          <t>BENNET, MICHAEL F.</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1073,31 +1073,31 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>GARY PAUL</t>
+          <t>FRED EYCHANER</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>BUTTIGIEG, PETE</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>GENINE FIDLER</t>
+          <t>FRED EYCHANER</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>HARRIS, KAMALA D.</t>
+          <t>KLOBUCHAR, AMY J.</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>GENINE FIDLER</t>
+          <t>FRED EYCHANER</t>
         </is>
       </c>
     </row>
@@ -1109,31 +1109,31 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>GERALD ACKER</t>
+          <t>GARY PAUL</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>BULLOCK, STEVE</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>GERALD ACKER</t>
+          <t>GENINE FIDLER</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>HARRIS, KAMALA D.</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>HENRY MUNOZ</t>
+          <t>GENINE FIDLER</t>
         </is>
       </c>
     </row>
@@ -1145,55 +1145,55 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>JAMES BREWSTER</t>
+          <t>GEORGE TSUNIS</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>DE BLASIO, BILL</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>JAMES COSTOS</t>
+          <t>GEORGE TSUNIS</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>BOOKER, CORY A.</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>JAMES COSTOS</t>
+          <t>GERALD ACKER</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>BUTTIGIEG, PETE</t>
+          <t>BULLOCK, STEVE</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>JAMES COSTOS</t>
+          <t>GERALD ACKER</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>BENNET, MICHAEL F.</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>JANE HARTLEY</t>
+          <t>HENRY MUNOZ</t>
         </is>
       </c>
     </row>
@@ -1205,50 +1205,50 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>JANE HARTLEY</t>
+          <t>JAMES BREWSTER</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>BUTTIGIEG, PETE</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>JANE HARTLEY</t>
+          <t>JAMES COSTOS</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>GILLIBRAND, KIRSTEN</t>
+          <t>BOOKER, CORY A.</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>JANE HARTLEY</t>
+          <t>JAMES COSTOS</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>HARRIS, KAMALA D.</t>
+          <t>BUTTIGIEG, PETE</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>JANE HARTLEY</t>
+          <t>JAMES COSTOS</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>HICKENLOOPER, JOHN W.</t>
+          <t>BENNET, MICHAEL F.</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -1260,7 +1260,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>KLOBUCHAR, AMY J.</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -1272,7 +1272,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>MOULTON, SETH</t>
+          <t>BUTTIGIEG, PETE</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -1284,7 +1284,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>O'ROURKE, BETO</t>
+          <t>GILLIBRAND, KIRSTEN</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -1296,60 +1296,60 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>HARRIS, KAMALA D.</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>JANE STETSON</t>
+          <t>JANE HARTLEY</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>BUTTIGIEG, PETE</t>
+          <t>HICKENLOOPER, JOHN W.</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>JANE STETSON</t>
+          <t>JANE HARTLEY</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>KLOBUCHAR, AMY J.</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>JANET KELLER</t>
+          <t>JANE HARTLEY</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>GILLIBRAND, KIRSTEN</t>
+          <t>MOULTON, SETH</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>JANET KELLER</t>
+          <t>JANE HARTLEY</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>HARRIS, KAMALA D.</t>
+          <t>O'ROURKE, BETO</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>JANET KELLER</t>
+          <t>JANE HARTLEY</t>
         </is>
       </c>
     </row>
@@ -1361,55 +1361,55 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>JAY SNYDER</t>
+          <t>JANE STETSON</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>BULLOCK, STEVE</t>
+          <t>BUTTIGIEG, PETE</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>JAY SNYDER</t>
+          <t>JANE STETSON</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>BUTTIGIEG, PETE</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>JAY SNYDER</t>
+          <t>JANET KELLER</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>KLOBUCHAR, AMY J.</t>
+          <t>GILLIBRAND, KIRSTEN</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>JAY SNYDER</t>
+          <t>JANET KELLER</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>BENNET, MICHAEL F.</t>
+          <t>HARRIS, KAMALA D.</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>JEFFREY KATZENBERG</t>
+          <t>JANET KELLER</t>
         </is>
       </c>
     </row>
@@ -1421,7 +1421,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>JEFFREY KATZENBERG</t>
+          <t>JAY SNYDER</t>
         </is>
       </c>
     </row>
@@ -1433,7 +1433,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>JEFFREY KATZENBERG</t>
+          <t>JAY SNYDER</t>
         </is>
       </c>
     </row>
@@ -1445,26 +1445,26 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>JEFFREY KATZENBERG</t>
+          <t>JAY SNYDER</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>CASTRO, JULIAN</t>
+          <t>KLOBUCHAR, AMY J.</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>JEFFREY KATZENBERG</t>
+          <t>JAY SNYDER</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>HICKENLOOPER, JOHN W.</t>
+          <t>BENNET, MICHAEL F.</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -1476,7 +1476,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>INSLEE, JAY R.</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -1488,7 +1488,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>KLOBUCHAR, AMY J.</t>
+          <t>BULLOCK, STEVE</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -1500,7 +1500,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>MOULTON, SETH</t>
+          <t>BUTTIGIEG, PETE</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -1512,7 +1512,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>O'ROURKE, BETO</t>
+          <t>CASTRO, JULIAN</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -1524,7 +1524,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>WARREN, ELIZABETH</t>
+          <t>HICKENLOOPER, JOHN W.</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -1536,72 +1536,72 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>BENNET, MICHAEL F.</t>
+          <t>INSLEE, JAY R.</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>JOHN EMERSON</t>
+          <t>JEFFREY KATZENBERG</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>KLOBUCHAR, AMY J.</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>JOHN EMERSON</t>
+          <t>JEFFREY KATZENBERG</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>GILLIBRAND, KIRSTEN</t>
+          <t>MOULTON, SETH</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>JOHN EMERSON</t>
+          <t>JEFFREY KATZENBERG</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>O'ROURKE, BETO</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>JOHN FRANK</t>
+          <t>JEFFREY KATZENBERG</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>WARREN, ELIZABETH</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>JOHN MORGAN</t>
+          <t>JEFFREY KATZENBERG</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>BULLOCK, STEVE</t>
+          <t>BENNET, MICHAEL F.</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>JOHN MORGAN</t>
+          <t>JOHN EMERSON</t>
         </is>
       </c>
     </row>
@@ -1613,19 +1613,19 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>JOHN PHILLIPS</t>
+          <t>JOHN EMERSON</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>BUTTIGIEG, PETE</t>
+          <t>GILLIBRAND, KIRSTEN</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>JOHN PHILLIPS</t>
+          <t>JOHN EMERSON</t>
         </is>
       </c>
     </row>
@@ -1637,7 +1637,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>JOSEPH FALK</t>
+          <t>JOHN FRANK</t>
         </is>
       </c>
     </row>
@@ -1649,19 +1649,19 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>JUSTIN TANNER</t>
+          <t>JOHN MORGAN</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>BENNET, MICHAEL F.</t>
+          <t>BULLOCK, STEVE</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>KEN SOLOMON</t>
+          <t>JOHN MORGAN</t>
         </is>
       </c>
     </row>
@@ -1673,55 +1673,55 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>KEN SOLOMON</t>
+          <t>JOHN PHILLIPS</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>BOOKER, CORY A.</t>
+          <t>BUTTIGIEG, PETE</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>KEN SOLOMON</t>
+          <t>JOHN PHILLIPS</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>BUTTIGIEG, PETE</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>KEN SOLOMON</t>
+          <t>JOSEPH FALK</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>HARRIS, KAMALA D.</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>KEN SOLOMON</t>
+          <t>JUSTIN TANNER</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>BENNET, MICHAEL F.</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>KRISTIN OBLANDER</t>
+          <t>KEN SOLOMON</t>
         </is>
       </c>
     </row>
@@ -1733,19 +1733,19 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>LENI ECCLES</t>
+          <t>KEN SOLOMON</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>BOOKER, CORY A.</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>LINDA MASON</t>
+          <t>KEN SOLOMON</t>
         </is>
       </c>
     </row>
@@ -1757,19 +1757,19 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>LINDA MASON</t>
+          <t>KEN SOLOMON</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>WARREN, ELIZABETH</t>
+          <t>HARRIS, KAMALA D.</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>LINDA MASON</t>
+          <t>KEN SOLOMON</t>
         </is>
       </c>
     </row>
@@ -1781,7 +1781,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>LOU FRILLMAN</t>
+          <t>KRISTIN OBLANDER</t>
         </is>
       </c>
     </row>
@@ -1793,103 +1793,103 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>MACK WILBOURN</t>
+          <t>LENI ECCLES</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>BOOKER, CORY A.</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>MACK WILBOURN</t>
+          <t>LINDA MASON</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>BENNET, MICHAEL F.</t>
+          <t>BUTTIGIEG, PETE</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>MARK GALLOGLY</t>
+          <t>LINDA MASON</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>WARREN, ELIZABETH</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>MARK GALLOGLY</t>
+          <t>LINDA MASON</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>BOOKER, CORY A.</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>MARK GALLOGLY</t>
+          <t>LOU FRILLMAN</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>HARRIS, KAMALA D.</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>MARK GALLOGLY</t>
+          <t>MACK WILBOURN</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>HICKENLOOPER, JOHN W.</t>
+          <t>BOOKER, CORY A.</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>MARK GALLOGLY</t>
+          <t>MACK WILBOURN</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>MOULTON, SETH</t>
+          <t>HARRIS, KAMALA D.</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>MARK GALLOGLY</t>
+          <t>MACK WILBOURN</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>BENNET, MICHAEL F.</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>MARK GILBERT</t>
+          <t>MARK GALLOGLY</t>
         </is>
       </c>
     </row>
@@ -1901,55 +1901,55 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>MARK NICHOLS</t>
+          <t>MARK GALLOGLY</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>BUTTIGIEG, PETE</t>
+          <t>BOOKER, CORY A.</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>MARK NICHOLS</t>
+          <t>MARK GALLOGLY</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>HARRIS, KAMALA D.</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>MASSI KIANI</t>
+          <t>MARK GALLOGLY</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>HICKENLOOPER, JOHN W.</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>MATTHEW BARZUN</t>
+          <t>MARK GALLOGLY</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>MOULTON, SETH</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>MATTIE MCFADDEN-LAWSON</t>
+          <t>MARK GALLOGLY</t>
         </is>
       </c>
     </row>
@@ -1961,31 +1961,31 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>MELLODY HOBSON</t>
+          <t>MARK GILBERT</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>BOOKER, CORY A.</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>MELLODY HOBSON</t>
+          <t>MARK NICHOLS</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>HICKENLOOPER, JOHN W.</t>
+          <t>BUTTIGIEG, PETE</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>MELLODY HOBSON</t>
+          <t>MARK NICHOLS</t>
         </is>
       </c>
     </row>
@@ -1997,31 +1997,31 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>MEREDITH DEWITT</t>
+          <t>MASSI KIANI</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>BOOKER, CORY A.</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>MEREDITH DEWITT</t>
+          <t>MATTHEW BARZUN</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>BUTTIGIEG, PETE</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>MEREDITH DEWITT</t>
+          <t>MATTIE MCFADDEN-LAWSON</t>
         </is>
       </c>
     </row>
@@ -2033,7 +2033,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>MICHAEL PARHAM</t>
+          <t>MELLODY HOBSON</t>
         </is>
       </c>
     </row>
@@ -2045,115 +2045,115 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>MICHAEL PARHAM</t>
+          <t>MELLODY HOBSON</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>HICKENLOOPER, JOHN W.</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>MICHAEL SMITH</t>
+          <t>MELLODY HOBSON</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>BOOKER, CORY A.</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>MICHAEL SMITH</t>
+          <t>MEREDITH DEWITT</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>BUTTIGIEG, PETE</t>
+          <t>BOOKER, CORY A.</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>MICHAEL SMITH</t>
+          <t>MEREDITH DEWITT</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>BUTTIGIEG, PETE</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>MITCHELL BERGER</t>
+          <t>MEREDITH DEWITT</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>BOOKER, CORY A.</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>MITCHELL BERGER</t>
+          <t>MICHAEL KEMPNER</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>BULLOCK, STEVE</t>
+          <t>BOOKER, CORY A.</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>MITCHELL BERGER</t>
+          <t>MICHAEL KEMPNER</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>HARRIS, KAMALA D.</t>
+          <t>BUTTIGIEG, PETE</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>MITCHELL BERGER</t>
+          <t>MICHAEL KEMPNER</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>KLOBUCHAR, AMY J.</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>MITCHELL BERGER</t>
+          <t>MICHAEL PARHAM</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>RYAN, TIMOTHY J.</t>
+          <t>BOOKER, CORY A.</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>MITCHELL BERGER</t>
+          <t>MICHAEL PARHAM</t>
         </is>
       </c>
     </row>
@@ -2165,103 +2165,103 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>NEIL BLUHM</t>
+          <t>MICHAEL SMITH</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>HICKENLOOPER, JOHN W.</t>
+          <t>BOOKER, CORY A.</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>NEIL BLUHM</t>
+          <t>MICHAEL SMITH</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>BUTTIGIEG, PETE</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>NOAH MAMET</t>
+          <t>MICHAEL SMITH</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>BOOKER, CORY A.</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>NOAH MAMET</t>
+          <t>MITCHELL BERGER</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>BENNET, MICHAEL F.</t>
+          <t>BOOKER, CORY A.</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>ORIN KRAMER</t>
+          <t>MITCHELL BERGER</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>BULLOCK, STEVE</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>ORIN KRAMER</t>
+          <t>MITCHELL BERGER</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>BULLOCK, STEVE</t>
+          <t>HARRIS, KAMALA D.</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>ORIN KRAMER</t>
+          <t>MITCHELL BERGER</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>KLOBUCHAR, AMY J.</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>PAM HAMAMOTO</t>
+          <t>MITCHELL BERGER</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>RYAN, TIMOTHY J.</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>RHONDA COHEN</t>
+          <t>MITCHELL BERGER</t>
         </is>
       </c>
     </row>
@@ -2273,19 +2273,19 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>RICHARD HARPOOTLIAN</t>
+          <t>NEIL BLUHM</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>HICKENLOOPER, JOHN W.</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>ROBERT POHLAD</t>
+          <t>NEIL BLUHM</t>
         </is>
       </c>
     </row>
@@ -2297,67 +2297,67 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>ROBERT WOLF</t>
+          <t>NOAH MAMET</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>HARRIS, KAMALA D.</t>
+          <t>BOOKER, CORY A.</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>ROBERT WOLF</t>
+          <t>NOAH MAMET</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>KLOBUCHAR, AMY J.</t>
+          <t>BENNET, MICHAEL F.</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>ROBERT WOLF</t>
+          <t>ORIN KRAMER</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>RYAN, TIMOTHY J.</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>ROBERT WOLF</t>
+          <t>ORIN KRAMER</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>BULLOCK, STEVE</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>RUSTY RUEFF</t>
+          <t>ORIN KRAMER</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>BOOKER, CORY A.</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>RUSTY RUEFF</t>
+          <t>PAM HAMAMOTO</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>SCOTT HARRIS</t>
+          <t>RHONDA COHEN</t>
         </is>
       </c>
     </row>
@@ -2381,7 +2381,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>SCOTT MILLER</t>
+          <t>RICHARD HARPOOTLIAN</t>
         </is>
       </c>
     </row>
@@ -2393,7 +2393,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>STEVE WESTLY</t>
+          <t>ROBERT POHLAD</t>
         </is>
       </c>
     </row>
@@ -2405,43 +2405,43 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>STEWART BAINUM</t>
+          <t>ROBERT WOLF</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>HARRIS, KAMALA D.</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>SUZI LEVINE</t>
+          <t>ROBERT WOLF</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>BOOKER, CORY A.</t>
+          <t>KLOBUCHAR, AMY J.</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>SUZI LEVINE</t>
+          <t>ROBERT WOLF</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>RYAN, TIMOTHY J.</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>TERENCE MCAULIFFE</t>
+          <t>ROBERT WOLF</t>
         </is>
       </c>
     </row>
@@ -2453,19 +2453,19 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>TIM BROAS</t>
+          <t>RUSTY RUEFF</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>BUTTIGIEG, PETE</t>
+          <t>BOOKER, CORY A.</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>TIM BROAS</t>
+          <t>RUSTY RUEFF</t>
         </is>
       </c>
     </row>
@@ -2477,7 +2477,7 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>TIM GILL</t>
+          <t>SCOTT HARRIS</t>
         </is>
       </c>
     </row>
@@ -2489,19 +2489,19 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>TOM FORD</t>
+          <t>SCOTT MILLER</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>BUTTIGIEG, PETE</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>TOM FORD</t>
+          <t>STEVE WESTLY</t>
         </is>
       </c>
     </row>
@@ -2513,7 +2513,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>TOM WHEELER</t>
+          <t>STEVEN GREEN</t>
         </is>
       </c>
     </row>
@@ -2525,31 +2525,31 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>WADE RANDLETT</t>
+          <t>STEWART BAINUM</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>SWALWELL, ERIC</t>
+          <t>BIDEN, JOSEPH R. JR.</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>WADE RANDLETT</t>
+          <t>SUZI LEVINE</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>BIDEN, JOSEPH R. JR.</t>
+          <t>BOOKER, CORY A.</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>WILLIAM FREEMAN</t>
+          <t>SUZI LEVINE</t>
         </is>
       </c>
     </row>
@@ -2560,6 +2560,126 @@
         </is>
       </c>
       <c r="B184" t="inlineStr">
+        <is>
+          <t>TERENCE MCAULIFFE</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>BIDEN, JOSEPH R. JR.</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>TIM BROAS</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>BUTTIGIEG, PETE</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>TIM BROAS</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>BIDEN, JOSEPH R. JR.</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>TIM GILL</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>BIDEN, JOSEPH R. JR.</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>TOM FORD</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>BUTTIGIEG, PETE</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>TOM FORD</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>BIDEN, JOSEPH R. JR.</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>TOM WHEELER</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>BIDEN, JOSEPH R. JR.</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>WADE RANDLETT</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>SWALWELL, ERIC</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>WADE RANDLETT</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>BIDEN, JOSEPH R. JR.</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>WILLIAM FREEMAN</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>BIDEN, JOSEPH R. JR.</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
         <is>
           <t>YOLANDA PARKER</t>
         </is>

</xml_diff>